<commit_message>
bow + f1 is done
</commit_message>
<xml_diff>
--- a/data/01_raw/data.xlsx
+++ b/data/01_raw/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>_unit_id</t>
   </si>
@@ -94,6 +94,99 @@
   </si>
   <si>
     <t>Apocalypse lighting. #Spokane #wildfires</t>
+  </si>
+  <si>
+    <t>#flood #disaster Heavy rain causes flash flooding of streets in Manitou, Colorado Springs areas</t>
+  </si>
+  <si>
+    <t>Typhoon Soudelor kills 28 in China and Taiwan</t>
+  </si>
+  <si>
+    <t>We're shaking...It's an earthquake</t>
+  </si>
+  <si>
+    <t>I'm on top of the hill and I can see a fire in the woods...</t>
+  </si>
+  <si>
+    <t>There's an emergency evacuation happening now in the building across the street</t>
+  </si>
+  <si>
+    <t>I'm afraid that the tornado is coming to our area...</t>
+  </si>
+  <si>
+    <t>Three people died from the heat wave so far</t>
+  </si>
+  <si>
+    <t>Haha South Tampa is getting flooded hah- WAIT A SECOND I LIVE IN SOUTH TAMPA WHAT AM I GONNA DO WHAT AM I GONNA DO FVCK #flooding</t>
+  </si>
+  <si>
+    <t>#raining #flooding #Florida #TampaBay #Tampa 18 or 19 days. I've lost count</t>
+  </si>
+  <si>
+    <t>#Flood in Bago Myanmar #We arrived Bago</t>
+  </si>
+  <si>
+    <t>Damage to school bus on 80 in multi car crash #BREAKING</t>
+  </si>
+  <si>
+    <t>Not Relevant</t>
+  </si>
+  <si>
+    <t>They'd probably still show more life than Arsenal did yesterday, eh? EH?</t>
+  </si>
+  <si>
+    <t>Hey! How are you?</t>
+  </si>
+  <si>
+    <t>What's up man?</t>
+  </si>
+  <si>
+    <t>I love fruits</t>
+  </si>
+  <si>
+    <t>Summer is lovely</t>
+  </si>
+  <si>
+    <t>My car is so fast</t>
+  </si>
+  <si>
+    <t>What a nice hat?</t>
+  </si>
+  <si>
+    <t>What a goooooooaaaaaal!!!!!!</t>
+  </si>
+  <si>
+    <t>Fuck off!</t>
+  </si>
+  <si>
+    <t>No I don't like cold!</t>
+  </si>
+  <si>
+    <t>this is ridiculous....</t>
+  </si>
+  <si>
+    <t>London is cool ;)</t>
+  </si>
+  <si>
+    <t>Love skiing</t>
+  </si>
+  <si>
+    <t>What a wonderful day!</t>
+  </si>
+  <si>
+    <t>NOOOOOOOOO! Don't do that!</t>
+  </si>
+  <si>
+    <t>LOOOOOOL</t>
+  </si>
+  <si>
+    <t>No way...I can't eat that shit</t>
+  </si>
+  <si>
+    <t>Was in NYC last week!</t>
+  </si>
+  <si>
+    <t>Love my girlfriend</t>
   </si>
 </sst>
 </file>
@@ -442,7 +535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,6 +944,1086 @@
       </c>
       <c r="N11" t="s"/>
     </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>778243835</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="n">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s"/>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s"/>
+      <c r="K12" t="s"/>
+      <c r="L12" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" t="n">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>778243836</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="n">
+        <v>157</v>
+      </c>
+      <c r="F13" t="s"/>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s"/>
+      <c r="K13" t="s"/>
+      <c r="L13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" t="n">
+        <v>12</v>
+      </c>
+      <c r="N13" t="s"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>778243837</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="n">
+        <v>143</v>
+      </c>
+      <c r="F14" t="s"/>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s"/>
+      <c r="K14" t="s"/>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" t="s"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>778243838</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="n">
+        <v>140</v>
+      </c>
+      <c r="F15" t="s"/>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.9607</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" t="s"/>
+      <c r="K15" t="s"/>
+      <c r="L15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" t="n">
+        <v>7</v>
+      </c>
+      <c r="N15" t="s"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>778243839</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="n">
+        <v>136</v>
+      </c>
+      <c r="F16" t="s"/>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.9215</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s"/>
+      <c r="K16" t="s"/>
+      <c r="L16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" t="n">
+        <v>8</v>
+      </c>
+      <c r="N16" t="s"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>778243840</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="n">
+        <v>147</v>
+      </c>
+      <c r="F17" t="s"/>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.7177</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s"/>
+      <c r="K17" t="s"/>
+      <c r="L17" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" t="n">
+        <v>9</v>
+      </c>
+      <c r="N17" t="s"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>778243841</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="n">
+        <v>147</v>
+      </c>
+      <c r="F18" t="s"/>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.9603</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s"/>
+      <c r="K18" t="s"/>
+      <c r="L18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M18" t="n">
+        <v>10</v>
+      </c>
+      <c r="N18" t="s"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>778243842</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="n">
+        <v>132</v>
+      </c>
+      <c r="F19" t="s"/>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s"/>
+      <c r="K19" t="s"/>
+      <c r="L19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" t="n">
+        <v>22</v>
+      </c>
+      <c r="N19" t="s"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>778243843</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="n">
+        <v>144</v>
+      </c>
+      <c r="F20" t="s"/>
+      <c r="G20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s"/>
+      <c r="K20" t="s"/>
+      <c r="L20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" t="n">
+        <v>23</v>
+      </c>
+      <c r="N20" t="s"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>778243844</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="n">
+        <v>147</v>
+      </c>
+      <c r="F21" t="s"/>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.6761</v>
+      </c>
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" t="s"/>
+      <c r="K21" t="s"/>
+      <c r="L21" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" t="n">
+        <v>24</v>
+      </c>
+      <c r="N21" t="s"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>778243845</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="n">
+        <v>136</v>
+      </c>
+      <c r="F22" t="s"/>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s"/>
+      <c r="K22" t="s"/>
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" t="n">
+        <v>25</v>
+      </c>
+      <c r="N22" t="s"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>778243846</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="n">
+        <v>151</v>
+      </c>
+      <c r="F23" t="s"/>
+      <c r="G23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.9612000000000001</v>
+      </c>
+      <c r="I23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s"/>
+      <c r="K23" t="s"/>
+      <c r="L23" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" t="n">
+        <v>26</v>
+      </c>
+      <c r="N23" t="s"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>778243847</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="n">
+        <v>124</v>
+      </c>
+      <c r="F24" t="s"/>
+      <c r="G24" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" t="s"/>
+      <c r="K24" t="s"/>
+      <c r="L24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" t="n">
+        <v>27</v>
+      </c>
+      <c r="N24" t="s"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>778243848</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="n">
+        <v>140</v>
+      </c>
+      <c r="F25" t="s"/>
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" t="s"/>
+      <c r="K25" t="s"/>
+      <c r="L25" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" t="n">
+        <v>28</v>
+      </c>
+      <c r="N25" t="s"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>778243849</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="n">
+        <v>141</v>
+      </c>
+      <c r="F26" t="s"/>
+      <c r="G26" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" t="s"/>
+      <c r="K26" t="s"/>
+      <c r="L26" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" t="n">
+        <v>29</v>
+      </c>
+      <c r="N26" t="s"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>778243851</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="n">
+        <v>142</v>
+      </c>
+      <c r="F27" t="s"/>
+      <c r="G27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s"/>
+      <c r="K27" t="s"/>
+      <c r="L27" t="s">
+        <v>42</v>
+      </c>
+      <c r="M27" t="n">
+        <v>30</v>
+      </c>
+      <c r="N27" t="s"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>778243852</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="n">
+        <v>138</v>
+      </c>
+      <c r="F28" t="s"/>
+      <c r="G28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s"/>
+      <c r="K28" t="s"/>
+      <c r="L28" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28" t="n">
+        <v>31</v>
+      </c>
+      <c r="N28" t="s"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>778243853</v>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="n">
+        <v>137</v>
+      </c>
+      <c r="F29" t="s"/>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" t="s"/>
+      <c r="K29" t="s"/>
+      <c r="L29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M29" t="n">
+        <v>32</v>
+      </c>
+      <c r="N29" t="s"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>778243855</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="n">
+        <v>143</v>
+      </c>
+      <c r="F30" t="s"/>
+      <c r="G30" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" t="s"/>
+      <c r="K30" t="s"/>
+      <c r="L30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" t="n">
+        <v>33</v>
+      </c>
+      <c r="N30" t="s"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>778243856</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="n">
+        <v>138</v>
+      </c>
+      <c r="F31" t="s"/>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" t="s"/>
+      <c r="K31" t="s"/>
+      <c r="L31" t="s">
+        <v>46</v>
+      </c>
+      <c r="M31" t="n">
+        <v>34</v>
+      </c>
+      <c r="N31" t="s"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>778243857</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="n">
+        <v>139</v>
+      </c>
+      <c r="F32" t="s"/>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" t="s"/>
+      <c r="K32" t="s"/>
+      <c r="L32" t="s">
+        <v>47</v>
+      </c>
+      <c r="M32" t="n">
+        <v>35</v>
+      </c>
+      <c r="N32" t="s"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>778243858</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="n">
+        <v>143</v>
+      </c>
+      <c r="F33" t="s"/>
+      <c r="G33" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" t="s"/>
+      <c r="K33" t="s"/>
+      <c r="L33" t="s">
+        <v>48</v>
+      </c>
+      <c r="M33" t="n">
+        <v>36</v>
+      </c>
+      <c r="N33" t="s"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>778243859</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="n">
+        <v>145</v>
+      </c>
+      <c r="F34" t="s"/>
+      <c r="G34" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" t="s"/>
+      <c r="K34" t="s"/>
+      <c r="L34" t="s">
+        <v>49</v>
+      </c>
+      <c r="M34" t="n">
+        <v>37</v>
+      </c>
+      <c r="N34" t="s"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>778243860</v>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="n">
+        <v>142</v>
+      </c>
+      <c r="F35" t="s"/>
+      <c r="G35" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" t="s"/>
+      <c r="K35" t="s"/>
+      <c r="L35" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" t="n">
+        <v>38</v>
+      </c>
+      <c r="N35" t="s"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>778243861</v>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="n">
+        <v>140</v>
+      </c>
+      <c r="F36" t="s"/>
+      <c r="G36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" t="s"/>
+      <c r="K36" t="s"/>
+      <c r="L36" t="s">
+        <v>51</v>
+      </c>
+      <c r="M36" t="n">
+        <v>39</v>
+      </c>
+      <c r="N36" t="s"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>778243863</v>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="n">
+        <v>141</v>
+      </c>
+      <c r="F37" t="s"/>
+      <c r="G37" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37" t="s"/>
+      <c r="K37" t="s"/>
+      <c r="L37" t="s">
+        <v>52</v>
+      </c>
+      <c r="M37" t="n">
+        <v>40</v>
+      </c>
+      <c r="N37" t="s"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>778243864</v>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="n">
+        <v>142</v>
+      </c>
+      <c r="F38" t="s"/>
+      <c r="G38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" t="s"/>
+      <c r="K38" t="s"/>
+      <c r="L38" t="s">
+        <v>53</v>
+      </c>
+      <c r="M38" t="n">
+        <v>41</v>
+      </c>
+      <c r="N38" t="s"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>778243865</v>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="n">
+        <v>150</v>
+      </c>
+      <c r="F39" t="s"/>
+      <c r="G39" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" t="s"/>
+      <c r="K39" t="s"/>
+      <c r="L39" t="s">
+        <v>54</v>
+      </c>
+      <c r="M39" t="n">
+        <v>42</v>
+      </c>
+      <c r="N39" t="s"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>778243866</v>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="n">
+        <v>147</v>
+      </c>
+      <c r="F40" t="s"/>
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" t="s"/>
+      <c r="K40" t="s"/>
+      <c r="L40" t="s">
+        <v>55</v>
+      </c>
+      <c r="M40" t="n">
+        <v>43</v>
+      </c>
+      <c r="N40" t="s"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>778243867</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="n">
+        <v>135</v>
+      </c>
+      <c r="F41" t="s"/>
+      <c r="G41" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>37</v>
+      </c>
+      <c r="J41" t="s"/>
+      <c r="K41" t="s"/>
+      <c r="L41" t="s">
+        <v>56</v>
+      </c>
+      <c r="M41" t="n">
+        <v>44</v>
+      </c>
+      <c r="N41" t="s"/>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>